<commit_message>
add login (fixes captcha, fix noavail products test crash)
</commit_message>
<xml_diff>
--- a/src/test/resources/book1.xlsx
+++ b/src/test/resources/book1.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>VC2184</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>12013896B</t>
   </si>
@@ -405,7 +402,7 @@
   <dimension ref="A1:A372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,13 +411,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="1">
+        <v>430206030</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -429,7 +426,9 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>430206030</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
fix empty single result table
</commit_message>
<xml_diff>
--- a/src/test/resources/book1.xlsx
+++ b/src/test/resources/book1.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>12013896B</t>
+  </si>
+  <si>
+    <t>L028011800R</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:A372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,8 +414,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>430206030</v>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>